<commit_message>
updated the PR schedule excel file
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahriar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A192F5-84DD-41D9-9F9E-855D332F7A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B523B3B7-D02D-46BB-B290-0293CF7E8FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -114,7 +114,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -454,7 +454,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +498,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="3">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Neural network is done and noted
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C754CD-D9BD-4A19-A87A-1F490CAF2BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB88EA6D-A42D-4E8A-A5F1-C137887A8EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
   <si>
     <t>Duration</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>NN</t>
-  </si>
-  <si>
-    <t>backprobagation formulas</t>
   </si>
 </sst>
 </file>
@@ -933,10 +930,10 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1559,14 +1556,12 @@
         <v>5</v>
       </c>
       <c r="F25" s="8">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="G25" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="28" t="s">
-        <v>42</v>
-      </c>
+      <c r="H25" s="28"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1579,9 +1574,7 @@
       <c r="D26" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>6</v>
-      </c>
+      <c r="E26" s="7"/>
       <c r="F26" s="8">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Bayesian Network subject done
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83DDFE3F-3FEF-4652-8A42-D0F4D6063595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AC59A8-87D8-4B5A-8954-344DD0326F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Duration</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>final slids</t>
+  </si>
+  <si>
+    <t>Bayesian Networks</t>
   </si>
 </sst>
 </file>
@@ -951,7 +954,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1685,17 +1688,21 @@
       <c r="B30" s="5">
         <v>28</v>
       </c>
-      <c r="C30" s="17">
+      <c r="C30" s="30">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F30" s="8">
-        <v>0</v>
-      </c>
-      <c r="G30" s="24"/>
+        <v>0.9</v>
+      </c>
+      <c r="G30" s="24" t="s">
+        <v>47</v>
+      </c>
       <c r="H30" s="25"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>

</xml_diff>

<commit_message>
Feature selection subject done
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481D6C83-E74A-4DFE-AFAC-68792F535068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310E02F-4B71-4F1B-A743-1D9A6AF4A262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -234,18 +234,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -482,26 +476,26 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -513,37 +507,37 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="5" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="6" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -564,16 +558,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -951,7 +942,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G31" sqref="G31"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="C32:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,10 +1577,10 @@
       <c r="B26" s="5">
         <v>24</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="26">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -1608,10 +1599,10 @@
       <c r="B27" s="5">
         <v>25</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="26">
         <v>0.12916666666666668</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -1633,10 +1624,10 @@
       <c r="B28" s="5">
         <v>26</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="26">
         <v>7.7777777777777779E-2</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1658,10 +1649,10 @@
       <c r="B29" s="5">
         <v>27</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="26">
         <v>2.9166666666666667E-2</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1685,10 +1676,10 @@
       <c r="B30" s="5">
         <v>28</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="26">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1710,10 +1701,10 @@
       <c r="B31" s="5">
         <v>29</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="26">
         <v>3.4027777777777775E-2</v>
       </c>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="27" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1735,10 +1726,10 @@
       <c r="B32" s="19">
         <v>30</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="28">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="28" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="20"/>

</xml_diff>

<commit_message>
Learning theory subject done; Also the course is finished. review is needed
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D310E02F-4B71-4F1B-A743-1D9A6AF4A262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798628BE-41C7-4A0A-912A-89E6D0A19368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
   <si>
     <t>Duration</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>Feature selection</t>
+  </si>
+  <si>
+    <t>final formulas</t>
+  </si>
+  <si>
+    <t>Learning Theory</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,9 +544,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -939,10 +942,10 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="C32:D32"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,10 +1004,10 @@
       <c r="F3" s="8">
         <v>0.9</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="23"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="9" t="s">
@@ -1030,10 +1033,10 @@
       <c r="F4" s="8">
         <v>0.9</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="23"/>
+      <c r="H4" s="22"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="11">
@@ -1059,10 +1062,10 @@
       <c r="F5" s="8">
         <v>0.9</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="23"/>
+      <c r="H5" s="22"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="13">
@@ -1088,10 +1091,10 @@
       <c r="F6" s="8">
         <v>0.9</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="23"/>
+      <c r="H6" s="22"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="13">
@@ -1117,10 +1120,10 @@
       <c r="F7" s="8">
         <v>0.9</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="23"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="15">
@@ -1146,10 +1149,10 @@
       <c r="F8" s="8">
         <v>0.9</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="23"/>
+      <c r="H8" s="22"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="17">
@@ -1175,10 +1178,10 @@
       <c r="F9" s="8">
         <v>0.9</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="23"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1200,10 +1203,10 @@
       <c r="F10" s="8">
         <v>0.9</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="23"/>
+      <c r="H10" s="22"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1225,10 +1228,10 @@
       <c r="F11" s="8">
         <v>0.9</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="23"/>
+      <c r="H11" s="22"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
@@ -1250,10 +1253,10 @@
       <c r="F12" s="8">
         <v>0.9</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="23"/>
+      <c r="H12" s="22"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1275,10 +1278,10 @@
       <c r="F13" s="8">
         <v>0.9</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="23"/>
+      <c r="H13" s="22"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
@@ -1300,10 +1303,10 @@
       <c r="F14" s="8">
         <v>0.9</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="23"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -1325,10 +1328,10 @@
       <c r="F15" s="8">
         <v>0.9</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="23"/>
+      <c r="H15" s="22"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
@@ -1350,10 +1353,10 @@
       <c r="F16" s="8">
         <v>0.9</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="22"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
@@ -1375,10 +1378,10 @@
       <c r="F17" s="8">
         <v>0.6</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="4"/>
@@ -1402,10 +1405,10 @@
       <c r="F18" s="8">
         <v>0.9</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="23"/>
+      <c r="H18" s="22"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1427,10 +1430,10 @@
       <c r="F19" s="8">
         <v>0.9</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="23"/>
+      <c r="H19" s="22"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1449,10 +1452,10 @@
       <c r="F20" s="8">
         <v>0.85</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H20" s="22" t="s">
         <v>14</v>
       </c>
       <c r="I20" s="4"/>
@@ -1473,10 +1476,10 @@
       <c r="F21" s="8">
         <v>0.9</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="22" t="s">
         <v>17</v>
       </c>
       <c r="I21" s="4"/>
@@ -1497,10 +1500,10 @@
       <c r="F22" s="8">
         <v>0.9</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="23"/>
+      <c r="H22" s="22"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1519,10 +1522,10 @@
       <c r="F23" s="8">
         <v>0.6</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I23" s="4"/>
@@ -1543,10 +1546,10 @@
       <c r="F24" s="8">
         <v>0.6</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="23" t="s">
+      <c r="H24" s="22" t="s">
         <v>20</v>
       </c>
       <c r="I24" s="4"/>
@@ -1567,20 +1570,20 @@
       <c r="F25" s="8">
         <v>0.9</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="H25" s="23"/>
+      <c r="H25" s="22"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="2:12" ht="18" x14ac:dyDescent="0.3">
       <c r="B26" s="5">
         <v>24</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="25">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="D26" s="27" t="s">
+      <c r="D26" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -1589,20 +1592,20 @@
       <c r="F26" s="8">
         <v>0.9</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H26" s="23"/>
+      <c r="H26" s="22"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="2:12" ht="18" x14ac:dyDescent="0.3">
       <c r="B27" s="5">
         <v>25</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="25">
         <v>0.12916666666666668</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -1611,10 +1614,10 @@
       <c r="F27" s="8">
         <v>0.9</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H27" s="23"/>
+      <c r="H27" s="22"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
@@ -1624,10 +1627,10 @@
       <c r="B28" s="5">
         <v>26</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <v>7.7777777777777779E-2</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1636,10 +1639,10 @@
       <c r="F28" s="8">
         <v>0.9</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H28" s="23"/>
+      <c r="H28" s="22"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1649,10 +1652,10 @@
       <c r="B29" s="5">
         <v>27</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
         <v>2.9166666666666667E-2</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="26" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1661,10 +1664,10 @@
       <c r="F29" s="8">
         <v>0.85</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="22" t="s">
         <v>46</v>
       </c>
       <c r="I29" s="4"/>
@@ -1676,10 +1679,10 @@
       <c r="B30" s="5">
         <v>28</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C30" s="25">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="26" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1688,10 +1691,10 @@
       <c r="F30" s="8">
         <v>0.9</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="23"/>
+      <c r="H30" s="22"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -1701,10 +1704,10 @@
       <c r="B31" s="5">
         <v>29</v>
       </c>
-      <c r="C31" s="26">
+      <c r="C31" s="25">
         <v>3.4027777777777775E-2</v>
       </c>
-      <c r="D31" s="27" t="s">
+      <c r="D31" s="26" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1713,10 +1716,10 @@
       <c r="F31" s="8">
         <v>0.9</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="H31" s="23"/>
+      <c r="H31" s="22"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
@@ -1726,18 +1729,24 @@
       <c r="B32" s="19">
         <v>30</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="27">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="21">
-        <v>0</v>
-      </c>
-      <c r="G32" s="24"/>
-      <c r="H32" s="25"/>
+      <c r="E32" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="20">
+        <v>0.85</v>
+      </c>
+      <c r="G32" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H32" s="24" t="s">
+        <v>49</v>
+      </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>

</xml_diff>

<commit_message>
working on last test of Ensemble learning
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798628BE-41C7-4A0A-912A-89E6D0A19368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB31C798-4EE8-4477-B418-A12F00CC4A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -487,7 +487,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,13 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -942,10 +936,10 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,7 +1441,7 @@
         <v>4</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F20" s="8">
         <v>0.85</v>
@@ -1580,10 +1574,10 @@
       <c r="B26" s="5">
         <v>24</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="6">
         <v>6.6666666666666666E-2</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E26" s="7" t="s">
@@ -1602,10 +1596,10 @@
       <c r="B27" s="5">
         <v>25</v>
       </c>
-      <c r="C27" s="25">
+      <c r="C27" s="6">
         <v>0.12916666666666668</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -1627,10 +1621,10 @@
       <c r="B28" s="5">
         <v>26</v>
       </c>
-      <c r="C28" s="25">
+      <c r="C28" s="6">
         <v>7.7777777777777779E-2</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E28" s="7" t="s">
@@ -1652,10 +1646,10 @@
       <c r="B29" s="5">
         <v>27</v>
       </c>
-      <c r="C29" s="25">
+      <c r="C29" s="6">
         <v>2.9166666666666667E-2</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="7" t="s">
         <v>6</v>
       </c>
       <c r="E29" s="7" t="s">
@@ -1679,10 +1673,10 @@
       <c r="B30" s="5">
         <v>28</v>
       </c>
-      <c r="C30" s="25">
+      <c r="C30" s="6">
         <v>3.4722222222222224E-2</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
@@ -1704,10 +1698,10 @@
       <c r="B31" s="5">
         <v>29</v>
       </c>
-      <c r="C31" s="25">
+      <c r="C31" s="6">
         <v>3.4027777777777775E-2</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E31" s="7" t="s">
@@ -1729,13 +1723,13 @@
       <c r="B32" s="19">
         <v>30</v>
       </c>
-      <c r="C32" s="27">
+      <c r="C32" s="25">
         <v>6.3194444444444442E-2</v>
       </c>
-      <c r="D32" s="27" t="s">
+      <c r="D32" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="25" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="20">

</xml_diff>

<commit_message>
last test of Ensemble learning done
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB31C798-4EE8-4477-B418-A12F00CC4A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E36D8C-8DD6-420F-AD1E-4464C078B2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>Duration</t>
   </si>
@@ -78,9 +78,6 @@
   </si>
   <si>
     <t>Problem</t>
-  </si>
-  <si>
-    <t>Last test</t>
   </si>
   <si>
     <t>Ensemble learning</t>
@@ -936,10 +933,10 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,16 +987,16 @@
         <v>4.791666666666667E-2</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G3" s="21" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>28</v>
       </c>
       <c r="H3" s="22"/>
       <c r="I3" s="4"/>
@@ -1008,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1019,16 +1016,16 @@
         <v>3.6805555555555557E-2</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="8">
         <v>0.9</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="4"/>
@@ -1037,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1048,16 +1045,16 @@
         <v>6.8750000000000006E-2</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="8">
         <v>0.9</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="4"/>
@@ -1066,7 +1063,7 @@
         <v>0.6</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1077,16 +1074,16 @@
         <v>5.347222222222222E-2</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="8">
         <v>0.9</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="4"/>
@@ -1095,7 +1092,7 @@
         <v>0.85</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1106,16 +1103,16 @@
         <v>0.05</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="8">
         <v>0.9</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="4"/>
@@ -1124,7 +1121,7 @@
         <v>0.9</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
@@ -1135,16 +1132,16 @@
         <v>0.05</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="8">
         <v>0.9</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="4"/>
@@ -1153,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="L8" s="18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1164,16 +1161,16 @@
         <v>2.2916666666666665E-2</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="8">
         <v>0.9</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="4"/>
@@ -1189,16 +1186,16 @@
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="8">
         <v>0.9</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="4"/>
@@ -1214,16 +1211,16 @@
         <v>5.7638888888888892E-2</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F11" s="8">
         <v>0.9</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="4"/>
@@ -1239,16 +1236,16 @@
         <v>3.0555555555555555E-2</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="8">
         <v>0.9</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="4"/>
@@ -1264,16 +1261,16 @@
         <v>0.05</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="8">
         <v>0.9</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="4"/>
@@ -1289,16 +1286,16 @@
         <v>6.458333333333334E-2</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14" s="8">
         <v>0.9</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="4"/>
@@ -1314,16 +1311,16 @@
         <v>2.8472222222222222E-2</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F15" s="8">
         <v>0.9</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="4"/>
@@ -1339,16 +1336,16 @@
         <v>5.1388888888888887E-2</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F16" s="8">
         <v>0.9</v>
       </c>
       <c r="G16" s="21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H16" s="22"/>
       <c r="I16" s="4"/>
@@ -1364,10 +1361,10 @@
         <v>6.3888888888888884E-2</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F17" s="8">
         <v>0.6</v>
@@ -1376,7 +1373,7 @@
         <v>9</v>
       </c>
       <c r="H17" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
@@ -1444,14 +1441,12 @@
         <v>7</v>
       </c>
       <c r="F20" s="8">
-        <v>0.85</v>
+        <v>0.9</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H20" s="22" t="s">
         <v>14</v>
       </c>
+      <c r="H20" s="22"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:12" ht="18" x14ac:dyDescent="0.3">
@@ -1471,10 +1466,10 @@
         <v>0.9</v>
       </c>
       <c r="G21" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="22" t="s">
         <v>16</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>17</v>
       </c>
       <c r="I21" s="4"/>
     </row>
@@ -1495,7 +1490,7 @@
         <v>0.9</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H22" s="22"/>
       <c r="I22" s="4"/>
@@ -1517,10 +1512,10 @@
         <v>0.6</v>
       </c>
       <c r="G23" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="H23" s="22" t="s">
-        <v>20</v>
       </c>
       <c r="I23" s="4"/>
     </row>
@@ -1541,10 +1536,10 @@
         <v>0.6</v>
       </c>
       <c r="G24" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="H24" s="22" t="s">
-        <v>20</v>
       </c>
       <c r="I24" s="4"/>
     </row>
@@ -1565,7 +1560,7 @@
         <v>0.9</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="4"/>
@@ -1587,7 +1582,7 @@
         <v>0.9</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="4"/>
@@ -1609,7 +1604,7 @@
         <v>0.9</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H27" s="22"/>
       <c r="I27" s="4"/>
@@ -1634,7 +1629,7 @@
         <v>0.9</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H28" s="22"/>
       <c r="I28" s="4"/>
@@ -1659,10 +1654,10 @@
         <v>0.85</v>
       </c>
       <c r="G29" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="22" t="s">
         <v>45</v>
-      </c>
-      <c r="H29" s="22" t="s">
-        <v>46</v>
       </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
@@ -1686,7 +1681,7 @@
         <v>0.9</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="4"/>
@@ -1711,7 +1706,7 @@
         <v>0.9</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="4"/>
@@ -1736,10 +1731,10 @@
         <v>0.85</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>

</xml_diff>

<commit_message>
reviewed the LDA but must focus on svm and markov
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\WarLog-2026.01.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45000469-A59F-4D12-9234-A6E36B31C650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC47E68-1D2F-487D-AAA3-866588F5539B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -936,10 +936,10 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
new color coding for the subjects focusing on completion
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A55568-E16F-4648-A66E-9762D0226115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ACE359-1EBE-44BB-96C0-C13215330EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="51">
   <si>
     <t>Duration</t>
   </si>
@@ -195,7 +195,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +235,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -480,14 +487,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -564,15 +572,49 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="3" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Accent3" xfId="4" builtinId="37"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -933,13 +975,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E97E6ABC-EF99-4767-B534-8AB459485FA1}">
-  <dimension ref="B1:L33"/>
+  <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,10 +994,12 @@
     <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -982,7 +1026,7 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -1010,8 +1054,14 @@
       <c r="L3" s="10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="N3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -1039,8 +1089,14 @@
       <c r="L4" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="N4" s="13">
+        <v>0.6</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -1068,8 +1124,14 @@
       <c r="L5" s="14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="N5" s="26">
+        <v>0.9</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -1099,8 +1161,14 @@
       <c r="L6" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+      <c r="N6" s="17">
+        <v>1</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -1129,7 +1197,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -1158,7 +1226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -1183,7 +1251,7 @@
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
     </row>
-    <row r="10" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -1208,7 +1276,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
     </row>
-    <row r="11" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -1233,7 +1301,7 @@
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
     </row>
-    <row r="12" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -1258,7 +1326,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
-    <row r="13" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -1283,7 +1351,7 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
     </row>
-    <row r="14" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -1308,7 +1376,7 @@
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -1333,7 +1401,7 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="2:12" ht="18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" ht="18" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>14</v>
       </c>
@@ -1757,14 +1825,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F32">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
-      <formula>0.9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
-      <formula>0.89</formula>
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
this topic holdout method and cross validation
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ACE359-1EBE-44BB-96C0-C13215330EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74203AA9-A9BC-49F1-A66C-77E190D2E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -584,68 +584,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -981,7 +920,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1145,7 +1084,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>30</v>
@@ -1182,7 +1121,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>30</v>
@@ -1211,7 +1150,7 @@
         <v>26</v>
       </c>
       <c r="F8" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>31</v>
@@ -1240,7 +1179,7 @@
         <v>26</v>
       </c>
       <c r="F9" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>32</v>
@@ -1265,7 +1204,7 @@
         <v>26</v>
       </c>
       <c r="F10" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>33</v>
@@ -1290,7 +1229,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>34</v>
@@ -1315,7 +1254,7 @@
         <v>26</v>
       </c>
       <c r="F12" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G12" s="21" t="s">
         <v>35</v>
@@ -1340,7 +1279,7 @@
         <v>26</v>
       </c>
       <c r="F13" s="8">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="G13" s="21" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
devised prompt for ml flashcards
</commit_message>
<xml_diff>
--- a/PatternRecognition-Schedule.xlsx
+++ b/PatternRecognition-Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Career\01. IE (Industrial Engineering)\00. Univesity\PHD\Exam Log\blackoutPhdPreparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D0978F-BA8A-4E80-A34B-A70122D52DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAF1B96-18B6-44E8-9647-FF8194231F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39CDB2C7-528F-45AA-A1B4-46CB04FC935A}"/>
   </bookViews>
@@ -917,10 +917,10 @@
   <dimension ref="B1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
+      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>